<commit_message>
update(file excel web ban hang)
</commit_message>
<xml_diff>
--- a/excel_web_ban_hang.xlsx
+++ b/excel_web_ban_hang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\j2team\doAnWeb\entity_relationship_diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00C785F9-0EFE-49CB-A947-EAFD20C58AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F0C70E-ABFE-4507-B1CF-E80F56790550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C74ADCA2-B6DE-4272-B19A-9D19ECD7EF21}"/>
   </bookViews>
@@ -102,19 +102,19 @@
     <t>Mã sản phẩm</t>
   </si>
   <si>
-    <t>Mã nhà sản xuất</t>
-  </si>
-  <si>
     <t>Số lượng</t>
   </si>
   <si>
-    <t>Giá mua</t>
-  </si>
-  <si>
     <t>Giá bán</t>
   </si>
   <si>
-    <t>Khuyến mãi</t>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Ảnh</t>
+  </si>
+  <si>
+    <t>Khuyến mãi(dựa vào số lượng mua)</t>
   </si>
 </sst>
 </file>
@@ -165,12 +165,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,17 +490,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA11DFE-4727-4A6A-831B-9388537F76DE}">
-  <dimension ref="B5:K28"/>
+  <dimension ref="B5:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:K23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
@@ -601,7 +604,7 @@
       <c r="E22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -609,7 +612,7 @@
       <c r="E23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -617,7 +620,7 @@
       <c r="E24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -625,25 +628,23 @@
       <c r="E25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E27" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>